<commit_message>
Removed extra local file
</commit_message>
<xml_diff>
--- a/covid_bhb.xlsx
+++ b/covid_bhb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u203711\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA3809\A29207215\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A29207215\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7264" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7309" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -594,7 +594,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -842,11 +842,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1675,6 +1677,115 @@
             </a:rPr>
             <a:t> also affect results for the following days.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>C10. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Figures on 30 November have been affected by a data processing issue. This means the figures for that day are lower than expected, and figures for 1 December slightly higher. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>C11. On 2 December, the 30 November figure for NHS Lanarkshire was revised down by 1, to remove a case reported from an LFT test. LFT tests will be reported separately by Public Health Scotland. The 1 December reported total had been adjusted at the time of publication to adjust for this case.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -2966,8 +3077,11 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>These were updated with the correct figures for that day on 26/11/20.</a:t>
+            <a:t>Number of confirmed covid patients in hospital was updated on 26/11/20 from 160 to 155, which changed the Scotland total from 1,161 to 1,156.</a:t>
           </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -3019,60 +3133,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>H19. On 28/11/2020, NHS Fife could not confirm figures, so previous day's figures were used.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>H20. On 29/11/2020, NHS Fife data for number of patients in hospital, was updated from 49 to 46. This changed Scotland total from 1,077 to 1,074.</a:t>
+            <a:t>H19. On 28/11/2020, NHS Fife could not confirm figures, so previous day's figures were used.  On 29/11/2020, the number of confirmed COVID patients in hospital was updated from 49 to 46, which changed the Scotland total from 1,077 to 1,074.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -7311,7 +7372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A46"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="M123" sqref="M123"/>
     </sheetView>
   </sheetViews>
@@ -7335,13 +7396,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:S271"/>
+  <dimension ref="A1:S274"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B259" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B266" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q277" sqref="Q277"/>
+      <selection pane="bottomRight" activeCell="C288" sqref="C288:C293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20148,7 +20209,7 @@
         <v>80135</v>
       </c>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>44150</v>
       </c>
@@ -20198,7 +20259,7 @@
         <v>81294</v>
       </c>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>44151</v>
       </c>
@@ -20248,7 +20309,7 @@
         <v>82011</v>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>44152</v>
       </c>
@@ -20298,7 +20359,7 @@
         <v>83259</v>
       </c>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>44153</v>
       </c>
@@ -20348,7 +20409,7 @@
         <v>84523</v>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>44154</v>
       </c>
@@ -20398,7 +20459,7 @@
         <v>85612</v>
       </c>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <v>44155</v>
       </c>
@@ -20448,7 +20509,7 @@
         <v>86630</v>
       </c>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>44156</v>
       </c>
@@ -20498,7 +20559,7 @@
         <v>87517</v>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>44157</v>
       </c>
@@ -20548,7 +20609,7 @@
         <v>88361</v>
       </c>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>44158</v>
       </c>
@@ -20598,7 +20659,7 @@
         <v>89310</v>
       </c>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>44159</v>
       </c>
@@ -20648,7 +20709,7 @@
         <v>90081</v>
       </c>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>44160</v>
       </c>
@@ -20698,7 +20759,7 @@
         <v>90961</v>
       </c>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <v>44161</v>
       </c>
@@ -20748,7 +20809,7 @@
         <v>92186</v>
       </c>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>44162</v>
       </c>
@@ -20798,7 +20859,7 @@
         <v>93155</v>
       </c>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <v>44163</v>
       </c>
@@ -20844,11 +20905,11 @@
       <c r="O270" s="122">
         <v>78</v>
       </c>
-      <c r="P270" s="128">
+      <c r="P270" s="127">
         <v>93943</v>
       </c>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>44164</v>
       </c>
@@ -20894,8 +20955,159 @@
       <c r="O271" s="122">
         <v>78</v>
       </c>
-      <c r="P271" s="128">
+      <c r="P271" s="127">
         <v>94689</v>
+      </c>
+    </row>
+    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A272" s="4">
+        <v>44165</v>
+      </c>
+      <c r="B272" s="122">
+        <v>6672</v>
+      </c>
+      <c r="C272" s="122">
+        <v>983</v>
+      </c>
+      <c r="D272" s="122">
+        <v>1143</v>
+      </c>
+      <c r="E272" s="122">
+        <v>4240</v>
+      </c>
+      <c r="F272" s="122">
+        <v>4120</v>
+      </c>
+      <c r="G272" s="122">
+        <v>4758</v>
+      </c>
+      <c r="H272" s="122">
+        <v>32703</v>
+      </c>
+      <c r="I272" s="122">
+        <v>1426</v>
+      </c>
+      <c r="J272" s="122">
+        <v>19461</v>
+      </c>
+      <c r="K272" s="122">
+        <v>13482</v>
+      </c>
+      <c r="L272" s="122">
+        <v>37</v>
+      </c>
+      <c r="M272" s="122">
+        <v>75</v>
+      </c>
+      <c r="N272" s="122">
+        <v>5879</v>
+      </c>
+      <c r="O272" s="122">
+        <v>78</v>
+      </c>
+      <c r="P272" s="127">
+        <v>95057</v>
+      </c>
+      <c r="R272" s="131"/>
+    </row>
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A273" s="4">
+        <v>44166</v>
+      </c>
+      <c r="B273" s="122">
+        <v>6716</v>
+      </c>
+      <c r="C273" s="122">
+        <v>994</v>
+      </c>
+      <c r="D273" s="122">
+        <v>1147</v>
+      </c>
+      <c r="E273" s="122">
+        <v>4300</v>
+      </c>
+      <c r="F273" s="122">
+        <v>4178</v>
+      </c>
+      <c r="G273" s="122">
+        <v>4801</v>
+      </c>
+      <c r="H273" s="122">
+        <v>32939</v>
+      </c>
+      <c r="I273" s="122">
+        <v>1433</v>
+      </c>
+      <c r="J273" s="122">
+        <v>19629</v>
+      </c>
+      <c r="K273" s="122">
+        <v>13565</v>
+      </c>
+      <c r="L273" s="122">
+        <v>38</v>
+      </c>
+      <c r="M273" s="122">
+        <v>75</v>
+      </c>
+      <c r="N273" s="122">
+        <v>5915</v>
+      </c>
+      <c r="O273" s="122">
+        <v>81</v>
+      </c>
+      <c r="P273" s="127">
+        <v>95811</v>
+      </c>
+    </row>
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A274" s="4">
+        <v>44167</v>
+      </c>
+      <c r="B274" s="122">
+        <v>6786</v>
+      </c>
+      <c r="C274" s="122">
+        <v>1000</v>
+      </c>
+      <c r="D274" s="122">
+        <v>1155</v>
+      </c>
+      <c r="E274" s="122">
+        <v>4369</v>
+      </c>
+      <c r="F274" s="122">
+        <v>4226</v>
+      </c>
+      <c r="G274" s="122">
+        <v>4864</v>
+      </c>
+      <c r="H274" s="122">
+        <v>33282</v>
+      </c>
+      <c r="I274" s="122">
+        <v>1445</v>
+      </c>
+      <c r="J274" s="122">
+        <v>19783</v>
+      </c>
+      <c r="K274" s="122">
+        <v>13680</v>
+      </c>
+      <c r="L274" s="122">
+        <v>38</v>
+      </c>
+      <c r="M274" s="122">
+        <v>75</v>
+      </c>
+      <c r="N274" s="122">
+        <v>5978</v>
+      </c>
+      <c r="O274" s="122">
+        <v>81</v>
+      </c>
+      <c r="P274" s="127">
+        <v>96762</v>
       </c>
     </row>
   </sheetData>
@@ -20910,18 +21122,18 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
+      <selection pane="bottomRight" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
     <col min="2" max="3" width="9.42578125" style="2"/>
     <col min="4" max="4" width="9.5703125" style="2" customWidth="1"/>
     <col min="5" max="7" width="9.42578125" style="2"/>
@@ -20932,28 +21144,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
       <c r="J1" s="37"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
     </row>
     <row r="3" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
@@ -25147,7 +25359,7 @@
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A82" s="127">
+      <c r="A82" s="130">
         <v>44163</v>
       </c>
       <c r="B82" s="99" t="s">
@@ -25200,7 +25412,7 @@
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A83" s="127">
+      <c r="A83" s="130">
         <v>44164</v>
       </c>
       <c r="B83" s="99" t="s">
@@ -25248,10 +25460,169 @@
       <c r="P83" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="Q83" s="129">
+      <c r="Q83" s="128">
         <v>76</v>
       </c>
-      <c r="R83" s="129"/>
+      <c r="R83" s="128"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84" s="130">
+        <v>44165</v>
+      </c>
+      <c r="B84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E84" s="2">
+        <v>6</v>
+      </c>
+      <c r="F84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G84" s="2">
+        <v>6</v>
+      </c>
+      <c r="H84" s="2">
+        <v>26</v>
+      </c>
+      <c r="I84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="J84" s="2">
+        <v>19</v>
+      </c>
+      <c r="K84" s="2">
+        <v>7</v>
+      </c>
+      <c r="L84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="M84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="N84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="O84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="P84" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q84" s="129">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85" s="36">
+        <v>44166</v>
+      </c>
+      <c r="B85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" s="2">
+        <v>5</v>
+      </c>
+      <c r="F85" s="2">
+        <v>5</v>
+      </c>
+      <c r="G85" s="2">
+        <v>6</v>
+      </c>
+      <c r="H85" s="2">
+        <v>25</v>
+      </c>
+      <c r="I85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="J85" s="2">
+        <v>16</v>
+      </c>
+      <c r="K85" s="2">
+        <v>6</v>
+      </c>
+      <c r="L85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="M85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="N85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="O85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="P85" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q85" s="100">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="36">
+        <v>44167</v>
+      </c>
+      <c r="B86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="D86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="E86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="F86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G86" s="2">
+        <v>6</v>
+      </c>
+      <c r="H86" s="2">
+        <v>22</v>
+      </c>
+      <c r="I86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="J86" s="2">
+        <v>17</v>
+      </c>
+      <c r="K86" s="2">
+        <v>5</v>
+      </c>
+      <c r="L86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="M86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="N86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="O86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="P86" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q86" s="100">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -25268,13 +25639,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J83" sqref="J83"/>
+      <selection pane="bottomRight" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25288,26 +25659,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
     </row>
     <row r="3" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
@@ -29604,6 +29975,165 @@
       </c>
       <c r="Q83" s="117">
         <v>1049</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" s="36">
+        <v>44165</v>
+      </c>
+      <c r="B84" s="2">
+        <v>95</v>
+      </c>
+      <c r="C84" s="2">
+        <v>9</v>
+      </c>
+      <c r="D84" s="2">
+        <v>5</v>
+      </c>
+      <c r="E84" s="2">
+        <v>38</v>
+      </c>
+      <c r="F84" s="2">
+        <v>25</v>
+      </c>
+      <c r="G84" s="2">
+        <v>54</v>
+      </c>
+      <c r="H84" s="2">
+        <v>375</v>
+      </c>
+      <c r="I84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="J84" s="2">
+        <v>231</v>
+      </c>
+      <c r="K84" s="2">
+        <v>134</v>
+      </c>
+      <c r="L84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="M84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="N84" s="2">
+        <v>71</v>
+      </c>
+      <c r="O84" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="P84" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q84" s="118">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" s="36">
+        <v>44166</v>
+      </c>
+      <c r="B85" s="2">
+        <v>95</v>
+      </c>
+      <c r="C85" s="2">
+        <v>11</v>
+      </c>
+      <c r="D85" s="2">
+        <v>5</v>
+      </c>
+      <c r="E85" s="2">
+        <v>36</v>
+      </c>
+      <c r="F85" s="2">
+        <v>27</v>
+      </c>
+      <c r="G85" s="2">
+        <v>58</v>
+      </c>
+      <c r="H85" s="2">
+        <v>364</v>
+      </c>
+      <c r="I85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="J85" s="2">
+        <v>217</v>
+      </c>
+      <c r="K85" s="2">
+        <v>132</v>
+      </c>
+      <c r="L85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="M85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="N85" s="2">
+        <v>72</v>
+      </c>
+      <c r="O85" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="P85" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q85" s="117">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="36">
+        <v>44167</v>
+      </c>
+      <c r="B86" s="2">
+        <v>95</v>
+      </c>
+      <c r="C86" s="2">
+        <v>10</v>
+      </c>
+      <c r="D86" s="2">
+        <v>5</v>
+      </c>
+      <c r="E86" s="2">
+        <v>31</v>
+      </c>
+      <c r="F86" s="2">
+        <v>27</v>
+      </c>
+      <c r="G86" s="2">
+        <v>56</v>
+      </c>
+      <c r="H86" s="2">
+        <v>359</v>
+      </c>
+      <c r="I86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="J86" s="2">
+        <v>206</v>
+      </c>
+      <c r="K86" s="2">
+        <v>128</v>
+      </c>
+      <c r="L86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="M86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="N86" s="2">
+        <v>69</v>
+      </c>
+      <c r="O86" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="P86" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q86" s="117">
+        <v>991</v>
       </c>
     </row>
   </sheetData>
@@ -29668,14 +30198,14 @@
       <c r="AI1" s="41"/>
     </row>
     <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
       <c r="S2" s="42" t="s">
         <v>27</v>
       </c>
@@ -61177,13 +61707,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-12-02T13:14:21Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-11-29T11:14:34Z</value>
+      <value order="0">2020-12-02T13:14:21Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -61195,16 +61725,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA45149703</value>
+      <value order="0">vA45229077</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">65.4</value>
+      <value order="0">67.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">444</value>
+      <value order="0">455</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>